<commit_message>
Version 2 - 01.06.2016
</commit_message>
<xml_diff>
--- a/Demo - Script/UserStories - Script.xlsx
+++ b/Demo - Script/UserStories - Script.xlsx
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -631,7 +631,7 @@
       <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6">
@@ -661,7 +661,7 @@
       <c r="F14" s="1">
         <v>9</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="6">

</xml_diff>

<commit_message>
Version 4 - 07.06.2016
</commit_message>
<xml_diff>
--- a/Demo - Script/UserStories - Script.xlsx
+++ b/Demo - Script/UserStories - Script.xlsx
@@ -77,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +197,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -498,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +596,7 @@
       <c r="F9" s="6">
         <v>9</v>
       </c>
-      <c r="G9" s="6"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
@@ -601,7 +611,7 @@
       <c r="F10" s="1">
         <v>4</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="6">
@@ -631,7 +641,7 @@
       <c r="F12" s="1">
         <v>3</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6">
@@ -646,7 +656,7 @@
       <c r="F13" s="6">
         <v>3</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="3:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1">

</xml_diff>